<commit_message>
Added multi-linear regression and additional data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/040e929440403464/Work/Career/Coding/Folio/ML/single_linear_regression/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/040e929440403464/Work/Career/Coding/Folio/ML/found_ml_projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82274551-984A-4224-873C-D968B53AB76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{82274551-984A-4224-873C-D968B53AB76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5468AA2C-10C0-4C00-8512-03DE41AE938A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7426840D-12DB-4AC1-9B31-CCE043ED04BF}"/>
+    <workbookView xWindow="-27630" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{7426840D-12DB-4AC1-9B31-CCE043ED04BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Address</t>
   </si>
@@ -85,6 +85,30 @@
   </si>
   <si>
     <t>78 Lord st</t>
+  </si>
+  <si>
+    <t>Bedrooms</t>
+  </si>
+  <si>
+    <t>Bathrooms</t>
+  </si>
+  <si>
+    <t>251 Stallwell st</t>
+  </si>
+  <si>
+    <t>307 Highett st</t>
+  </si>
+  <si>
+    <t>27 Bennett st</t>
+  </si>
+  <si>
+    <t>66 Duke st</t>
+  </si>
+  <si>
+    <t>25 Beissel st</t>
+  </si>
+  <si>
+    <t>355 Burnley st</t>
   </si>
 </sst>
 </file>
@@ -452,22 +476,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AC86B1-8EF4-4C6E-8A94-C56ADDFB9018}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,10 +513,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -509,12 +541,18 @@
       <c r="F2" s="3">
         <v>192</v>
       </c>
-      <c r="G2" s="4">
-        <f t="shared" ref="G2:G13" si="0">IFERROR(D2/F2,"")</f>
+      <c r="G2" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <f t="shared" ref="I2:I19" si="0">IFERROR(D2/F2,"")</f>
         <v>6515.625</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -533,12 +571,18 @@
       <c r="F3" s="3">
         <v>234</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
         <f t="shared" si="0"/>
         <v>5064.1025641025644</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -557,12 +601,18 @@
       <c r="F4" s="3">
         <v>126</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
         <f t="shared" si="0"/>
         <v>9126.9841269841272</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -581,12 +631,18 @@
       <c r="F5" s="3">
         <v>219</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
         <f t="shared" si="0"/>
         <v>5410.9589041095887</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -605,12 +661,18 @@
       <c r="F6" s="3">
         <v>183</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
         <f t="shared" si="0"/>
         <v>7103.8251366120221</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -629,12 +691,18 @@
       <c r="F7">
         <v>122</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>8811.4754098360663</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -653,12 +721,18 @@
       <c r="F8" s="3">
         <v>175</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
         <f t="shared" si="0"/>
         <v>7028.5714285714284</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -677,12 +751,18 @@
       <c r="F9">
         <v>181</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
         <f t="shared" si="0"/>
         <v>7182.3204419889498</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -701,12 +781,18 @@
       <c r="F10" s="3">
         <v>152</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
         <f t="shared" si="0"/>
         <v>7539.4736842105267</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -725,12 +811,18 @@
       <c r="F11" s="3">
         <v>135</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
         <f t="shared" si="0"/>
         <v>8148.1481481481478</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -749,12 +841,18 @@
       <c r="F12" s="3">
         <v>142</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
         <f t="shared" si="0"/>
         <v>8070.422535211268</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -773,9 +871,195 @@
       <c r="F13" s="3">
         <v>123</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
         <f t="shared" si="0"/>
         <v>8943.0894308943098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45668</v>
+      </c>
+      <c r="D14" s="2">
+        <v>880000</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>148</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>5945.9459459459458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45643</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>151</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>6622.5165562913908</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45639</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1550000</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>164</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
+        <v>9451.2195121951227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45636</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1380000</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>165</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="0"/>
+        <v>8363.636363636364</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45633</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2354000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>309</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="0"/>
+        <v>7618.1229773462783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45626</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1950000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>213</v>
+      </c>
+      <c r="G19" s="3">
+        <v>4</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
+        <v>9154.929577464789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>